<commit_message>
working google maps api
</commit_message>
<xml_diff>
--- a/2025 Code/Blue/Captcha/lidar_images.xlsx
+++ b/2025 Code/Blue/Captcha/lidar_images.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1113,296 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>008.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>006.jpg</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>003.jpg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>004.jpg</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>pipeline_debug.jpg</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>